<commit_message>
Updated scripts with new API, using Financial Modeling Prep, now; finalized WACC calculation
</commit_message>
<xml_diff>
--- a/data/dax_40_stocks.xlsx
+++ b/data/dax_40_stocks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\svens\00_SST\Programming\00_Data_Science_Projects\Finance\20220908_ValuationModel\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D88C73-118B-4482-B2CF-008C6E33EE9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C44A83-69AB-4605-ACE8-6F3DE03DEC36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" xr2:uid="{292872DA-BD30-465C-A5FE-974159122087}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="182">
   <si>
     <t>Mercedes-Benz Group</t>
   </si>
@@ -456,6 +456,129 @@
   </si>
   <si>
     <t>ZAL.DE</t>
+  </si>
+  <si>
+    <t>shortname</t>
+  </si>
+  <si>
+    <t>ADIDAS AG</t>
+  </si>
+  <si>
+    <t>AIRBUS SE</t>
+  </si>
+  <si>
+    <t>ALLIANZ SE</t>
+  </si>
+  <si>
+    <t>BASF SE</t>
+  </si>
+  <si>
+    <t>BAYER AG</t>
+  </si>
+  <si>
+    <t>BEIERSDORF AG O.N.</t>
+  </si>
+  <si>
+    <t>BAYERISCHE MOTOREN WERKE AG</t>
+  </si>
+  <si>
+    <t>BRENNTAG SE NA O.N.</t>
+  </si>
+  <si>
+    <t>CONTINENTAL AG</t>
+  </si>
+  <si>
+    <t>COVESTRO AG</t>
+  </si>
+  <si>
+    <t>Delivery Hero SE Namens-Aktien</t>
+  </si>
+  <si>
+    <t>DEUTSCHE BANK AG</t>
+  </si>
+  <si>
+    <t>DEUTSCHE BOERSE NA O.N.</t>
+  </si>
+  <si>
+    <t>DEUTSCHE POST AG</t>
+  </si>
+  <si>
+    <t>DEUTSCHE TELEKOM AG</t>
+  </si>
+  <si>
+    <t>E.ON SE</t>
+  </si>
+  <si>
+    <t>FRESENIUS MEDICAL CARE AG &amp; CO</t>
+  </si>
+  <si>
+    <t>FRESENIUS SE&amp;CO KGAA</t>
+  </si>
+  <si>
+    <t>HEIDELBERGCEMENT AG O.N.</t>
+  </si>
+  <si>
+    <t>HELLOFRESH SE INH O.N.</t>
+  </si>
+  <si>
+    <t>HENKEL AG&amp;CO. KGAA</t>
+  </si>
+  <si>
+    <t>INFINEON TECHNOLOGIES AG</t>
+  </si>
+  <si>
+    <t>LINDE PLC EO 0,001</t>
+  </si>
+  <si>
+    <t>MERCEDES-BENZ GROUP</t>
+  </si>
+  <si>
+    <t>MERCK KGAA</t>
+  </si>
+  <si>
+    <t>MTU AERO ENGINES NA O.N.</t>
+  </si>
+  <si>
+    <t>MUENCHENER RUECKVERSICHERUNGS A</t>
+  </si>
+  <si>
+    <t>PORSCHE AUTOM.HLDG VZO</t>
+  </si>
+  <si>
+    <t>PUMA SE</t>
+  </si>
+  <si>
+    <t>Qiagen N.V.</t>
+  </si>
+  <si>
+    <t>RWE AG INH O.N.</t>
+  </si>
+  <si>
+    <t>SAP SE</t>
+  </si>
+  <si>
+    <t>SARTORIUS AG VZO O.N.</t>
+  </si>
+  <si>
+    <t>SIEMENS AG</t>
+  </si>
+  <si>
+    <t>SIEMENS ENERGY AG NA O.N.</t>
+  </si>
+  <si>
+    <t>SIEMENS HEALTH.AG NA O.N.</t>
+  </si>
+  <si>
+    <t>SYMRISE AG INH. O.N.</t>
+  </si>
+  <si>
+    <t>VOLKSWAGEN AG</t>
+  </si>
+  <si>
+    <t>VONOVIA SE NA O.N.</t>
+  </si>
+  <si>
+    <t>ZALANDO SE</t>
   </si>
 </sst>
 </file>
@@ -816,10 +939,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6C7306E-42B1-4EAE-97C4-72C824A20C93}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -827,7 +950,7 @@
     <col min="1" max="1" width="18.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>98</v>
       </c>
@@ -840,8 +963,11 @@
       <c r="D1" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F1" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -854,8 +980,11 @@
       <c r="D2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -868,8 +997,11 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -882,8 +1014,11 @@
       <c r="D4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -896,8 +1031,11 @@
       <c r="D5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -910,8 +1048,11 @@
       <c r="D6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -924,8 +1065,11 @@
       <c r="D7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -938,8 +1082,11 @@
       <c r="D8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -952,8 +1099,11 @@
       <c r="D9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F9" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -966,8 +1116,11 @@
       <c r="D10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -980,8 +1133,11 @@
       <c r="D11" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -994,8 +1150,11 @@
       <c r="D12" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -1008,8 +1167,11 @@
       <c r="D13" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F13" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -1022,8 +1184,11 @@
       <c r="D14" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F14" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -1036,8 +1201,11 @@
       <c r="D15" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F15" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -1050,8 +1218,11 @@
       <c r="D16" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -1064,8 +1235,11 @@
       <c r="D17" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F17" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -1078,8 +1252,11 @@
       <c r="D18" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F18" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -1092,8 +1269,11 @@
       <c r="D19" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -1106,8 +1286,11 @@
       <c r="D20" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F20" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -1120,8 +1303,11 @@
       <c r="D21" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F21" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>54</v>
       </c>
@@ -1134,8 +1320,11 @@
       <c r="D22" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F22" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -1148,8 +1337,11 @@
       <c r="D23" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F23" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>59</v>
       </c>
@@ -1162,8 +1354,11 @@
       <c r="D24" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F24" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -1176,8 +1371,11 @@
       <c r="D25" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F25" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>62</v>
       </c>
@@ -1190,8 +1388,11 @@
       <c r="D26" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F26" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>64</v>
       </c>
@@ -1204,8 +1405,11 @@
       <c r="D27" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F27" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -1218,8 +1422,11 @@
       <c r="D28" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F28" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>67</v>
       </c>
@@ -1232,8 +1439,11 @@
       <c r="D29" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F29" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>69</v>
       </c>
@@ -1246,8 +1456,11 @@
       <c r="D30" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F30" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>71</v>
       </c>
@@ -1260,8 +1473,11 @@
       <c r="D31" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F31" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>74</v>
       </c>
@@ -1274,8 +1490,11 @@
       <c r="D32" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F32" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>77</v>
       </c>
@@ -1288,8 +1507,11 @@
       <c r="D33" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F33" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>80</v>
       </c>
@@ -1302,8 +1524,11 @@
       <c r="D34" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F34" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>82</v>
       </c>
@@ -1316,8 +1541,11 @@
       <c r="D35" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F35" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>84</v>
       </c>
@@ -1330,8 +1558,11 @@
       <c r="D36" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F36" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>87</v>
       </c>
@@ -1344,8 +1575,11 @@
       <c r="D37" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F37" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -1358,8 +1592,11 @@
       <c r="D38" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F38" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>91</v>
       </c>
@@ -1372,8 +1609,11 @@
       <c r="D39" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F39" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>93</v>
       </c>
@@ -1386,8 +1626,11 @@
       <c r="D40" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F40" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>96</v>
       </c>
@@ -1399,6 +1642,9 @@
       </c>
       <c r="D41" t="s">
         <v>31</v>
+      </c>
+      <c r="F41" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>